<commit_message>
new variable works fine and a controller to download the excel is also added
</commit_message>
<xml_diff>
--- a/src/main/resources/timesheet.xlsx
+++ b/src/main/resources/timesheet.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Krishna\Birmingham\code\atm\src\main\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="3900" yWindow="825" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
@@ -26,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="44">
   <si>
     <t>DATE</t>
   </si>
@@ -85,9 +80,6 @@
     <t>3hrs</t>
   </si>
   <si>
-    <t xml:space="preserve">WEEKLY TOTAL </t>
-  </si>
-  <si>
     <t>EmpID</t>
   </si>
   <si>
@@ -146,6 +138,21 @@
   </si>
   <si>
     <t>-----</t>
+  </si>
+  <si>
+    <t>SUPERVIOSR NAME</t>
+  </si>
+  <si>
+    <t>COST CENTRE</t>
+  </si>
+  <si>
+    <t>SCHOOL NAME</t>
+  </si>
+  <si>
+    <t>START DATE</t>
+  </si>
+  <si>
+    <t>ADDED</t>
   </si>
 </sst>
 </file>
@@ -414,7 +421,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -449,7 +456,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -658,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,16 +680,20 @@
     <col min="6" max="6" width="18" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.140625" customWidth="1"/>
     <col min="11" max="11" width="18.28515625" customWidth="1"/>
-    <col min="12" max="12" width="12" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.28515625" customWidth="1"/>
-    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>4</v>
@@ -720,13 +731,25 @@
       <c r="M1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="N1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>12</v>
@@ -762,21 +785,21 @@
         <v>17</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="C3" s="5">
         <v>41497</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>15</v>
@@ -800,33 +823,33 @@
         <v>0</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" s="5">
         <v>41579</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="H4" s="1">
         <v>2013</v>
@@ -841,15 +864,15 @@
         <v>0</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>12</v>
@@ -864,10 +887,10 @@
         <v>15</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H5" s="1">
         <v>2013</v>
@@ -888,18 +911,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="5">
         <v>41585</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>15</v>
@@ -908,7 +931,7 @@
         <v>14</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H6" s="1">
         <v>2013</v>
@@ -923,15 +946,15 @@
         <v>0</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>12</v>
@@ -949,7 +972,7 @@
         <v>14</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H7" s="1">
         <v>2013</v>
@@ -967,30 +990,30 @@
         <v>17</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="C8" s="5">
         <v>41589</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H8" s="1">
         <v>2013</v>
@@ -1005,33 +1028,33 @@
         <v>0</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="5">
         <v>41589</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H9" s="1">
         <v>2013</v>
@@ -1046,15 +1069,15 @@
         <v>0</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>12</v>
@@ -1069,10 +1092,10 @@
         <v>15</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H10" s="1">
         <v>2013</v>
@@ -1093,27 +1116,27 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="5">
         <v>41596</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H11" s="1">
         <v>2013</v>
@@ -1128,33 +1151,33 @@
         <v>0</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M11" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="C12" s="5">
         <v>41596</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H12" s="1">
         <v>2013</v>
@@ -1169,15 +1192,15 @@
         <v>0</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>12</v>
@@ -1192,10 +1215,10 @@
         <v>15</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H13" s="1">
         <v>2013</v>
@@ -1216,9 +1239,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>12</v>
@@ -1233,10 +1256,10 @@
         <v>15</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H14" s="1">
         <v>2013</v>
@@ -1257,27 +1280,27 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="C15" s="5">
         <v>41590</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H15" s="1">
         <v>2013</v>
@@ -1292,33 +1315,33 @@
         <v>0</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>22</v>
       </c>
       <c r="C16" s="10">
         <v>41590</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>15</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H16" s="7">
         <v>2013</v>
@@ -1333,7 +1356,7 @@
         <v>0</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M16" s="7" t="s">
         <v>18</v>
@@ -1341,25 +1364,25 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17" s="5">
         <v>41590</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H17" s="1">
         <v>2013</v>
@@ -1374,20 +1397,20 @@
         <v>0</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>